<commit_message>
- more mutant analysis with botium (TBC)
</commit_message>
<xml_diff>
--- a/mutation-analysis/mutants-rasa/results_pizza.xlsx
+++ b/mutation-analysis/mutants-rasa/results_pizza.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proyectos\satori\user-simulator-evaluation\mutation-analysis\mutants-rasa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8CA0860-BAA2-4CBA-B98A-BC09B2C149F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8EE87FF-C662-44E8-907D-7E5C5492DFAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{30994DF1-0BCB-424C-A5E9-BD42686768CC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="108">
   <si>
     <t>mutant_DA_001</t>
   </si>
@@ -345,6 +345,21 @@
   </si>
   <si>
     <t>se borra la respuesta de toppings, así que esos 7 tests dan timeout</t>
+  </si>
+  <si>
+    <t>#tests = 52</t>
+  </si>
+  <si>
+    <t>KILLED</t>
+  </si>
+  <si>
+    <t>Hace que salte un intent distinto (expected toppings but found order drinks)</t>
+  </si>
+  <si>
+    <t>Hace que salte un intent distinto</t>
+  </si>
+  <si>
+    <t>Mut Score</t>
   </si>
 </sst>
 </file>
@@ -388,7 +403,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -411,15 +426,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -756,10 +785,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D0D3457-99EE-4908-9FC8-7C7A14894CA8}">
-  <dimension ref="A1:F94"/>
+  <dimension ref="A1:I94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,9 +796,10 @@
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="6" max="6" width="65.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>93</v>
       </c>
@@ -788,8 +818,11 @@
       <c r="F1" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -805,7 +838,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -815,7 +848,7 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -824,8 +857,15 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>107</v>
+      </c>
+      <c r="I4">
+        <f>COUNTIF(E2:E94, "Killed")/(COUNTIF(E2:E94, "Killed")+COUNTIF(E2:E94, "survived"))</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -839,7 +879,7 @@
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -849,7 +889,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -859,7 +899,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -869,7 +909,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -879,7 +919,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -889,7 +929,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -899,7 +939,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -913,7 +953,7 @@
       </c>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -923,7 +963,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -933,7 +973,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -943,7 +983,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -1051,10 +1091,14 @@
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="1"/>
+      <c r="B26" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
+      <c r="E26" s="1" t="s">
+        <v>101</v>
+      </c>
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1071,50 +1115,74 @@
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="1"/>
+      <c r="B28" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
+      <c r="E28" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="1"/>
+      <c r="B29" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
+      <c r="E29" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="1"/>
+      <c r="B30" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
+      <c r="E30" s="1" t="s">
+        <v>101</v>
+      </c>
       <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="1"/>
+      <c r="B31" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
+      <c r="E31" s="1" t="s">
+        <v>101</v>
+      </c>
       <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="1"/>
+      <c r="B32" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
+      <c r="E32" s="1" t="s">
+        <v>101</v>
+      </c>
       <c r="F32" s="1"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
- Finished mutation analysis of Botium tests with pizza-shop (15 mutants)
</commit_message>
<xml_diff>
--- a/mutation-analysis/mutants-rasa/results_pizza.xlsx
+++ b/mutation-analysis/mutants-rasa/results_pizza.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proyectos\satori\user-simulator-evaluation\mutation-analysis\mutants-rasa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8EE87FF-C662-44E8-907D-7E5C5492DFAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB0CAFE1-B117-45A6-93EE-9276F1D67F03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{30994DF1-0BCB-424C-A5E9-BD42686768CC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="108">
   <si>
     <t>mutant_DA_001</t>
   </si>
@@ -338,18 +338,12 @@
     <t>Done</t>
   </si>
   <si>
-    <t>Killed</t>
-  </si>
-  <si>
     <t>survived</t>
   </si>
   <si>
     <t>se borra la respuesta de toppings, así que esos 7 tests dan timeout</t>
   </si>
   <si>
-    <t>#tests = 52</t>
-  </si>
-  <si>
     <t>KILLED</t>
   </si>
   <si>
@@ -359,7 +353,13 @@
     <t>Hace que salte un intent distinto</t>
   </si>
   <si>
-    <t>Mut Score</t>
+    <t>Mut Score Botium</t>
+  </si>
+  <si>
+    <t>Botium # tests = 52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mutantes = </t>
   </si>
 </sst>
 </file>
@@ -441,7 +441,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -451,6 +451,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -788,7 +789,7 @@
   <dimension ref="A1:I94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,6 +798,7 @@
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
     <col min="6" max="6" width="65.7109375" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -818,9 +820,7 @@
       <c r="F1" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>103</v>
-      </c>
+      <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -832,10 +832,17 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
+      </c>
+      <c r="H2" t="s">
+        <v>107</v>
+      </c>
+      <c r="I2" s="5">
+        <f>(COUNTIF(E2:E94, "Killed")+COUNTIF(E2:E94, "survived"))</f>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -847,6 +854,9 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
+      <c r="H3" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -858,11 +868,11 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="H4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I4">
         <f>COUNTIF(E2:E94, "Killed")/(COUNTIF(E2:E94, "Killed")+COUNTIF(E2:E94, "survived"))</f>
-        <v>0.3</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -875,7 +885,7 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F5" s="1"/>
     </row>
@@ -949,7 +959,7 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F12" s="1"/>
     </row>
@@ -1053,7 +1063,7 @@
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F22" s="1"/>
     </row>
@@ -1097,7 +1107,7 @@
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F26" s="1"/>
     </row>
@@ -1121,10 +1131,10 @@
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1137,10 +1147,10 @@
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1153,7 +1163,7 @@
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F30" s="1"/>
     </row>
@@ -1167,7 +1177,7 @@
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F31" s="1"/>
     </row>
@@ -1181,7 +1191,7 @@
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F32" s="1"/>
     </row>
@@ -1189,10 +1199,14 @@
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="1"/>
+      <c r="B33" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
+      <c r="E33" s="1" t="s">
+        <v>100</v>
+      </c>
       <c r="F33" s="1"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1219,10 +1233,14 @@
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="1"/>
+      <c r="B36" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
+      <c r="E36" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="F36" s="1"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1249,10 +1267,14 @@
       <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B39" s="1"/>
+      <c r="B39" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
+      <c r="E39" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="F39" s="1"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1369,10 +1391,14 @@
       <c r="A51" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B51" s="1"/>
+      <c r="B51" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
+      <c r="E51" s="1" t="s">
+        <v>100</v>
+      </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -1739,11 +1765,15 @@
       <c r="A88" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B88" s="1"/>
+      <c r="B88" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
-      <c r="E88" s="1"/>
-      <c r="F88" s="2"/>
+      <c r="E88" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F88" s="1"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">

</xml_diff>